<commit_message>
Multimedia and Spreadsheet Data, script files
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AliceInWonderlandCharacter.xlsx
+++ b/data/Spreadsheet_Data/AliceInWonderlandCharacter.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D0A827-315C-4941-8A47-F68F508A4E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="40" yWindow="500" windowWidth="53340" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -14,12 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>hasId</t>
-  </si>
-  <si>
-    <t>hasAliceInWonderlandCharacterType</t>
-  </si>
-  <si>
-    <t>hasAliceInWonderlandCharacterDescription</t>
   </si>
   <si>
     <t>hasAliceInWonderlandSymbol</t>
@@ -235,27 +238,43 @@
   <si>
     <t>W_024</t>
   </si>
+  <si>
+    <t>hasDescription</t>
+  </si>
+  <si>
+    <t>hasName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -264,39 +283,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -486,270 +517,275 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="32.25"/>
-    <col customWidth="1" min="3" max="3" width="46.75"/>
-    <col customWidth="1" min="4" max="4" width="24.88"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="179.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="126" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="168" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="126" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="182" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="238" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="140" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="140" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="18" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update data and data model
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AliceInWonderlandCharacter.xlsx
+++ b/data/Spreadsheet_Data/AliceInWonderlandCharacter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8551D6-D96E-2847-B80F-28FF99A84994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCDCA97-2624-0142-B5D6-501C473EC66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34380" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13520" yWindow="5240" windowWidth="51780" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
-  <si>
-    <t>hasId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>W_001</t>
   </si>
@@ -203,18 +200,6 @@
     <t>W_019</t>
   </si>
   <si>
-    <t>hasDescription</t>
-  </si>
-  <si>
-    <t>hasName</t>
-  </si>
-  <si>
-    <t>linkToImageID</t>
-  </si>
-  <si>
-    <t>linkToLocationID</t>
-  </si>
-  <si>
     <t>Alice's sister</t>
   </si>
   <si>
@@ -225,13 +210,313 @@
   </si>
   <si>
     <t>Knave of Hearts</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Link to Image ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Link to Location ID</t>
+  </si>
+  <si>
+    <r>
+      <t>The Dormouse sat between the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>March Hare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> and the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mad Hatter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. They were using him as a cushion while he slept when </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> arrives at the start of the chapter.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Knave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> of Hearts is mentioned first in chapter 8, and later in chapters 11 and 12, which deal with his trial for a tart burglary in which the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>King of Hearts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> presides as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>judge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Alice eventually defends the Knave after the evidence becomes increasingly absurd and she is called as a witness.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>This character is the sister of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>Alice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>, implied to be the elder as Alice is referred to as, "this same little sister of hers". Her character is likely a fictionalized counterpart to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lorina Charlotte "Ina" Liddell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t> (1849-1930), the real-life elder sister of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>Alice Liddell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t> who was also inspiration for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>the Lory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t> at the Caucus Race.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When compared to the Queen of Hearts, the King of Hearts appears to be the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>moderate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> part of the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wonderland</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> government. As an example, when the Queen, who enjoys ordering </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>beheadings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, attempts to have Alice executed (charged with being unable to answer who is lying down in front of her), the King of Hearts reminds her that she is only a child.</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1]</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -239,42 +524,63 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="14"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color rgb="FF202122"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,19 +606,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,239 +839,281 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B19:B20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="3"/>
+    <col min="2" max="2" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="171" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="228" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="152" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="247" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="323" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="190" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="76" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="171" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="76" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="252" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="358" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="238" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="306" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="397" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="252" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="126" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="84" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="266" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="140" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>57</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>